<commit_message>
Result Figure Code Done
</commit_message>
<xml_diff>
--- a/foundPath/10000pathNodes.xlsx
+++ b/foundPath/10000pathNodes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="76" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="72" uniqueCount="4">
   <si>
     <t>X</t>
   </si>
@@ -70,7 +70,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -157,41 +157,41 @@
         <v>890</v>
       </c>
       <c r="B6" s="0">
-        <v>740</v>
+        <v>680</v>
       </c>
       <c r="C6" s="0">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D6" s="0">
-        <v>8.0896686159844062</v>
+        <v>5.3445705767687191</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="B7" s="0">
-        <v>820</v>
+        <v>690</v>
       </c>
       <c r="C7" s="0">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D7" s="0">
-        <v>10.777087865417259</v>
+        <v>5.8708863662424031</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="B8" s="0">
-        <v>870</v>
+        <v>720</v>
       </c>
       <c r="C8" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D8" s="0">
-        <v>12.29223938056877</v>
+        <v>7.2345227298787664</v>
       </c>
     </row>
     <row r="9">
@@ -199,279 +199,279 @@
         <v>890</v>
       </c>
       <c r="B9" s="0">
-        <v>920</v>
+        <v>740</v>
       </c>
       <c r="C9" s="0">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="0">
-        <v>14.02072057161717</v>
+        <v>8.0345227298787663</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>860</v>
+        <v>890</v>
       </c>
       <c r="B10" s="0">
-        <v>980</v>
+        <v>850</v>
       </c>
       <c r="C10" s="0">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D10" s="0">
-        <v>16.600799007193849</v>
+        <v>11.64108010692795</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>850</v>
+        <v>890</v>
       </c>
       <c r="B11" s="0">
-        <v>990</v>
+        <v>890</v>
       </c>
       <c r="C11" s="0">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D11" s="0">
-        <v>17.243623353727081</v>
+        <v>12.835109957674209</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>840</v>
+        <v>870</v>
       </c>
       <c r="B12" s="0">
-        <v>1000</v>
+        <v>970</v>
       </c>
       <c r="C12" s="0">
-        <v>21</v>
+        <v>24.043348177281938</v>
       </c>
       <c r="D12" s="0">
-        <v>17.95073013491362</v>
+        <v>15.77790745976138</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>820</v>
+        <v>860</v>
       </c>
       <c r="B13" s="0">
-        <v>1000</v>
+        <v>980</v>
       </c>
       <c r="C13" s="0">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D13" s="0">
-        <v>19.76891195309544</v>
+        <v>16.46703913404124</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>800</v>
+        <v>830</v>
       </c>
       <c r="B14" s="0">
-        <v>990</v>
+        <v>1000</v>
       </c>
       <c r="C14" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14" s="0">
-        <v>23.20901653386435</v>
+        <v>19.13781785660716</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>790</v>
+        <v>820</v>
       </c>
       <c r="B15" s="0">
-        <v>980</v>
+        <v>1000</v>
       </c>
       <c r="C15" s="0">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D15" s="0">
-        <v>24.2565821356222</v>
+        <v>20.007383073998469</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>760</v>
+        <v>800</v>
       </c>
       <c r="B16" s="0">
-        <v>930</v>
+        <v>990</v>
       </c>
       <c r="C16" s="0">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D16" s="0">
-        <v>27.32550418554078</v>
+        <v>21.49809505899832</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>730</v>
+        <v>760</v>
       </c>
       <c r="B17" s="0">
-        <v>870</v>
+        <v>950</v>
       </c>
       <c r="C17" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="0">
-        <v>30.063546606969091</v>
+        <v>24.191835177804219</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>710</v>
+        <v>720</v>
       </c>
       <c r="B18" s="0">
-        <v>850</v>
+        <v>860</v>
       </c>
       <c r="C18" s="0">
-        <v>23</v>
+        <v>20.338293528939332</v>
       </c>
       <c r="D18" s="0">
-        <v>31.218006657885901</v>
+        <v>28.536444132047109</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>640</v>
+        <v>700</v>
       </c>
       <c r="B19" s="0">
-        <v>830</v>
+        <v>840</v>
       </c>
       <c r="C19" s="0">
-        <v>15.17368524526475</v>
+        <v>23</v>
       </c>
       <c r="D19" s="0">
-        <v>35.032209998488753</v>
+        <v>29.8417226256996</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>620</v>
+        <v>680</v>
       </c>
       <c r="B20" s="0">
         <v>830</v>
       </c>
       <c r="C20" s="0">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D20" s="0">
-        <v>36.275462044223453</v>
+        <v>30.75440343284237</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>570</v>
+        <v>670</v>
       </c>
       <c r="B21" s="0">
-        <v>850</v>
+        <v>830</v>
       </c>
       <c r="C21" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="0">
-        <v>39.109759311136351</v>
+        <v>31.189186041538029</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>520</v>
+        <v>590</v>
       </c>
       <c r="B22" s="0">
-        <v>880</v>
+        <v>860</v>
       </c>
       <c r="C22" s="0">
-        <v>17</v>
+        <v>25.011964829212861</v>
       </c>
       <c r="D22" s="0">
-        <v>42.178681361054927</v>
+        <v>34.985511653066297</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>490</v>
+        <v>570</v>
       </c>
       <c r="B23" s="0">
-        <v>890</v>
+        <v>870</v>
       </c>
       <c r="C23" s="0">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D23" s="0">
-        <v>44.038844690565739</v>
+        <v>35.829120443913297</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>460</v>
+        <v>550</v>
       </c>
       <c r="B24" s="0">
-        <v>890</v>
+        <v>880</v>
       </c>
       <c r="C24" s="0">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D24" s="0">
-        <v>45.974328561533483</v>
+        <v>36.600178367189088</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>430</v>
+        <v>500</v>
       </c>
       <c r="B25" s="0">
-        <v>870</v>
+        <v>900</v>
       </c>
       <c r="C25" s="0">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D25" s="0">
-        <v>49.109590540197821</v>
+        <v>38.457131748959597</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>420</v>
+        <v>490</v>
       </c>
       <c r="B26" s="0">
-        <v>850</v>
+        <v>900</v>
       </c>
       <c r="C26" s="0">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D26" s="0">
-        <v>50.972980521447653</v>
+        <v>38.873798415626268</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>420</v>
+        <v>440</v>
       </c>
       <c r="B27" s="0">
-        <v>840</v>
+        <v>880</v>
       </c>
       <c r="C27" s="0">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D27" s="0">
-        <v>51.597980521447653</v>
+        <v>41.321600600687397</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>420</v>
+        <v>430</v>
       </c>
       <c r="B28" s="0">
-        <v>830</v>
+        <v>870</v>
       </c>
       <c r="C28" s="0">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D28" s="0">
-        <v>52.153536077003203</v>
+        <v>41.923393605952548</v>
       </c>
     </row>
     <row r="29">
@@ -479,13 +479,13 @@
         <v>420</v>
       </c>
       <c r="B29" s="0">
-        <v>820</v>
+        <v>830</v>
       </c>
       <c r="C29" s="0">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D29" s="0">
-        <v>52.653536077003203</v>
+        <v>43.886777237199063</v>
       </c>
     </row>
     <row r="30">
@@ -493,629 +493,447 @@
         <v>420</v>
       </c>
       <c r="B30" s="0">
-        <v>720</v>
+        <v>820</v>
       </c>
       <c r="C30" s="0">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D30" s="0">
-        <v>56.427120982663581</v>
+        <v>44.386777237199063</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>450</v>
+        <v>420</v>
       </c>
       <c r="B31" s="0">
-        <v>640</v>
+        <v>780</v>
       </c>
       <c r="C31" s="0">
-        <v>22.727959804814699</v>
+        <v>23</v>
       </c>
       <c r="D31" s="0">
-        <v>59.549475178138593</v>
+        <v>46.204959055380883</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>500</v>
+        <v>440</v>
       </c>
       <c r="B32" s="0">
-        <v>580</v>
+        <v>710</v>
       </c>
       <c r="C32" s="0">
-        <v>23.889310335394061</v>
+        <v>28</v>
       </c>
       <c r="D32" s="0">
-        <v>62.900271847448522</v>
+        <v>49.059904110000687</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>540</v>
+        <v>470</v>
       </c>
       <c r="B33" s="0">
-        <v>500</v>
+        <v>650</v>
       </c>
       <c r="C33" s="0">
-        <v>23</v>
+        <v>27.90418795780726</v>
       </c>
       <c r="D33" s="0">
-        <v>66.71532984084692</v>
+        <v>51.45979727634532</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>550</v>
+        <v>520</v>
       </c>
       <c r="B34" s="0">
-        <v>460</v>
+        <v>560</v>
       </c>
       <c r="C34" s="0">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D34" s="0">
-        <v>68.63305338764583</v>
+        <v>54.733229610578057</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>550</v>
+        <v>560</v>
       </c>
       <c r="B35" s="0">
-        <v>450</v>
+        <v>460</v>
       </c>
       <c r="C35" s="0">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D35" s="0">
-        <v>69.120858265694608</v>
+        <v>57.900973614774827</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>540</v>
+        <v>550</v>
       </c>
       <c r="B36" s="0">
-        <v>440</v>
+        <v>420</v>
       </c>
       <c r="C36" s="0">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D36" s="0">
-        <v>70.406506958761057</v>
+        <v>59.693628234608603</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>520</v>
+        <v>540</v>
       </c>
       <c r="B37" s="0">
-        <v>430</v>
+        <v>410</v>
       </c>
       <c r="C37" s="0">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D37" s="0">
-        <v>73.84661153952996</v>
+        <v>60.668947932796939</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>500</v>
+        <v>520</v>
       </c>
       <c r="B38" s="0">
-        <v>430</v>
+        <v>400</v>
       </c>
       <c r="C38" s="0">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D38" s="0">
-        <v>75.27518296810139</v>
+        <v>61.911207920296818</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>490</v>
+        <v>450</v>
       </c>
       <c r="B39" s="0">
-        <v>430</v>
+        <v>390</v>
       </c>
       <c r="C39" s="0">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D39" s="0">
-        <v>75.863418262219042</v>
+        <v>65.125329652962947</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>480</v>
+        <v>390</v>
       </c>
       <c r="B40" s="0">
-        <v>430</v>
+        <v>390</v>
       </c>
       <c r="C40" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D40" s="0">
-        <v>76.389734051692727</v>
+        <v>67.307147834781134</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>460</v>
+        <v>340</v>
       </c>
       <c r="B41" s="0">
-        <v>430</v>
+        <v>390</v>
       </c>
       <c r="C41" s="0">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D41" s="0">
-        <v>77.319966609832264</v>
+        <v>68.799685148213968</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>430</v>
+        <v>320</v>
       </c>
       <c r="B42" s="0">
-        <v>430</v>
+        <v>380</v>
       </c>
       <c r="C42" s="0">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D42" s="0">
-        <v>78.519966609832267</v>
+        <v>69.598280854463894</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>390</v>
+        <v>310</v>
       </c>
       <c r="B43" s="0">
-        <v>420</v>
+        <v>360</v>
       </c>
       <c r="C43" s="0">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D43" s="0">
-        <v>80.04704276746844</v>
+        <v>70.995823340401259</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="B44" s="0">
-        <v>380</v>
+        <v>330</v>
       </c>
       <c r="C44" s="0">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D44" s="0">
-        <v>83.147911132198658</v>
+        <v>72.995823340401259</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="B45" s="0">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="C45" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D45" s="0">
-        <v>85.473492527547492</v>
+        <v>73.522139129874944</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>280</v>
+        <v>330</v>
       </c>
       <c r="B46" s="0">
-        <v>320</v>
+        <v>270</v>
       </c>
       <c r="C46" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D46" s="0">
-        <v>86.788826631959139</v>
+        <v>76.086503323748516</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>280</v>
+        <v>370</v>
       </c>
       <c r="B47" s="0">
-        <v>310</v>
+        <v>220</v>
       </c>
       <c r="C47" s="0">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D47" s="0">
-        <v>87.529567372699887</v>
+        <v>78.700023420659889</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>300</v>
+        <v>420</v>
       </c>
       <c r="B48" s="0">
-        <v>270</v>
+        <v>190</v>
       </c>
       <c r="C48" s="0">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D48" s="0">
-        <v>90.723950197699594</v>
+        <v>80.986671222560005</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>310</v>
+        <v>460</v>
       </c>
       <c r="B49" s="0">
-        <v>260</v>
+        <v>180</v>
       </c>
       <c r="C49" s="0">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D49" s="0">
-        <v>91.50962439901798</v>
+        <v>82.669571477914147</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>340</v>
+        <v>570</v>
       </c>
       <c r="B50" s="0">
-        <v>240</v>
+        <v>170</v>
       </c>
       <c r="C50" s="0">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D50" s="0">
-        <v>93.186624992257052</v>
+        <v>86.54513674710266</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>360</v>
+        <v>580</v>
       </c>
       <c r="B51" s="0">
-        <v>230</v>
+        <v>170</v>
       </c>
       <c r="C51" s="0">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D51" s="0">
-        <v>94.063514395198141</v>
+        <v>86.852829054794967</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>400</v>
+        <v>670</v>
       </c>
       <c r="B52" s="0">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="C52" s="0">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D52" s="0">
-        <v>95.579492685028512</v>
+        <v>89.665329054794967</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>460</v>
+        <v>720</v>
       </c>
       <c r="B53" s="0">
         <v>180</v>
       </c>
       <c r="C53" s="0">
-        <v>28</v>
+        <v>32.203385853539821</v>
       </c>
       <c r="D53" s="0">
-        <v>97.815560662528299</v>
+        <v>91.278856382400065</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>490</v>
+        <v>810</v>
       </c>
       <c r="B54" s="0">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="C54" s="0">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D54" s="0">
-        <v>99.202311153091372</v>
+        <v>94.446900413547155</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>510</v>
+        <v>840</v>
       </c>
       <c r="B55" s="0">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="C55" s="0">
-        <v>26</v>
+        <v>24.541242364689118</v>
       </c>
       <c r="D55" s="0">
-        <v>100.09673834409131</v>
+        <v>95.873676292718272</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>550</v>
+        <v>870</v>
       </c>
       <c r="B56" s="0">
-        <v>140</v>
+        <v>260</v>
       </c>
       <c r="C56" s="0">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D56" s="0">
-        <v>101.65262725941869</v>
+        <v>97.933780136964828</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>610</v>
+        <v>890</v>
       </c>
       <c r="B57" s="0">
-        <v>140</v>
+        <v>310</v>
       </c>
       <c r="C57" s="0">
-        <v>28.523339139620909</v>
+        <v>29</v>
       </c>
       <c r="D57" s="0">
-        <v>103.8138805604539</v>
+        <v>99.965917800034447</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>720</v>
+        <v>900</v>
       </c>
       <c r="B58" s="0">
-        <v>150</v>
+        <v>340</v>
       </c>
       <c r="C58" s="0">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D58" s="0">
-        <v>107.34707669782649</v>
+        <v>101.0027301476306</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>780</v>
+        <v>910</v>
       </c>
       <c r="B59" s="0">
-        <v>170</v>
+        <v>430</v>
       </c>
       <c r="C59" s="0">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D59" s="0">
-        <v>109.35487203761591</v>
+        <v>103.8774555883092</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>860</v>
+        <v>910</v>
       </c>
       <c r="B60" s="0">
-        <v>230</v>
+        <v>480</v>
       </c>
       <c r="C60" s="0">
-        <v>24.61337882406934</v>
+        <v>33</v>
       </c>
       <c r="D60" s="0">
-        <v>113.0852841919458</v>
+        <v>105.4399555883092</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>870</v>
+        <v>900</v>
       </c>
       <c r="B61" s="0">
-        <v>240</v>
+        <v>530</v>
       </c>
       <c r="C61" s="0">
-        <v>26</v>
+        <v>30.235014617601159</v>
       </c>
       <c r="D61" s="0">
-        <v>113.6441141279154</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="0">
-        <v>890</v>
-      </c>
-      <c r="B62" s="0">
-        <v>280</v>
-      </c>
-      <c r="C62" s="0">
-        <v>21.296581491482279</v>
-      </c>
-      <c r="D62" s="0">
-        <v>115.53521738061249</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="0">
-        <v>910</v>
-      </c>
-      <c r="B63" s="0">
-        <v>350</v>
-      </c>
-      <c r="C63" s="0">
-        <v>28</v>
-      </c>
-      <c r="D63" s="0">
-        <v>118.4888136215763</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="0">
-        <v>920</v>
-      </c>
-      <c r="B64" s="0">
-        <v>410</v>
-      </c>
-      <c r="C64" s="0">
-        <v>30</v>
-      </c>
-      <c r="D64" s="0">
-        <v>120.58631794236879</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="0">
-        <v>940</v>
-      </c>
-      <c r="B65" s="0">
-        <v>530</v>
-      </c>
-      <c r="C65" s="0">
-        <v>34</v>
-      </c>
-      <c r="D65" s="0">
-        <v>124.38804452380521</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="0">
-        <v>900</v>
-      </c>
-      <c r="B66" s="0">
-        <v>520</v>
-      </c>
-      <c r="C66" s="0">
-        <v>21.62096934546506</v>
-      </c>
-      <c r="D66" s="0">
-        <v>124.9204450728009</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="0">
-        <v>870</v>
-      </c>
-      <c r="B67" s="0">
-        <v>460</v>
-      </c>
-      <c r="C67" s="0">
-        <v>38</v>
-      </c>
-      <c r="D67" s="0">
-        <v>119.2488156138824</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="0">
-        <v>870</v>
-      </c>
-      <c r="B68" s="0">
-        <v>480</v>
-      </c>
-      <c r="C68" s="0">
-        <v>40</v>
-      </c>
-      <c r="D68" s="0">
-        <v>119.7616361267029</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="0">
-        <v>880</v>
-      </c>
-      <c r="B69" s="0">
-        <v>520</v>
-      </c>
-      <c r="C69" s="0">
-        <v>25</v>
-      </c>
-      <c r="D69" s="0">
-        <v>121.0302840115083</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="0">
-        <v>870</v>
-      </c>
-      <c r="B70" s="0">
-        <v>370</v>
-      </c>
-      <c r="C70" s="0">
-        <v>41</v>
-      </c>
-      <c r="D70" s="0">
-        <v>97.272267533445302</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="0">
-        <v>870</v>
-      </c>
-      <c r="B71" s="0">
-        <v>390</v>
-      </c>
-      <c r="C71" s="0">
-        <v>41</v>
-      </c>
-      <c r="D71" s="0">
-        <v>97.760072411494079</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="0">
-        <v>870</v>
-      </c>
-      <c r="B72" s="0">
-        <v>410</v>
-      </c>
-      <c r="C72" s="0">
-        <v>41</v>
-      </c>
-      <c r="D72" s="0">
-        <v>98.247877289542856</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="0">
-        <v>870</v>
-      </c>
-      <c r="B73" s="0">
-        <v>430</v>
-      </c>
-      <c r="C73" s="0">
-        <v>41</v>
-      </c>
-      <c r="D73" s="0">
-        <v>98.735682167591634</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="0">
-        <v>880</v>
-      </c>
-      <c r="B74" s="0">
-        <v>520</v>
-      </c>
-      <c r="C74" s="0">
-        <v>36.984545227590402</v>
-      </c>
-      <c r="D74" s="0">
-        <v>101.05803593953711</v>
+        <v>107.0526758650191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>